<commit_message>
Add Agriwebb module and transition Auth2 Flow
</commit_message>
<xml_diff>
--- a/table_mapping.xlsx
+++ b/table_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amir\PycharmProjects\agriwebb-experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D78EA4-BD96-4709-9A17-8C6EE2715743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1DB11C-FDD7-46BD-94BB-71938C56512C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="83">
   <si>
     <t>AnimalRecord</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Ranchforce</t>
   </si>
   <si>
-    <t>FeatureFlagGlobal</t>
-  </si>
-  <si>
     <t>Pasture</t>
   </si>
   <si>
@@ -133,9 +130,6 @@
     <t>BoundaryDataHistoryPasture</t>
   </si>
   <si>
-    <t>PaddockDataHistoryPasture,</t>
-  </si>
-  <si>
     <t>PastureCropDesignerSetting</t>
   </si>
   <si>
@@ -145,9 +139,6 @@
     <t>PaddockDataHistoryPasture</t>
   </si>
   <si>
-    <t>Last Models Created</t>
-  </si>
-  <si>
     <t>PastureSoilSampleData</t>
   </si>
   <si>
@@ -221,6 +212,66 @@
   </si>
   <si>
     <t>ArvaUserPastureSharingRequest</t>
+  </si>
+  <si>
+    <t>No Json Variable</t>
+  </si>
+  <si>
+    <t>No Data</t>
+  </si>
+  <si>
+    <t>No Json Variable/ but it store geometry data</t>
+  </si>
+  <si>
+    <t>json fields (practisec,recommendations,prefered_program_ids,avoided_programs_ids)</t>
+  </si>
+  <si>
+    <t>no data for looking inside json fields for variables</t>
+  </si>
+  <si>
+    <t>no json field</t>
+  </si>
+  <si>
+    <t>json fields(data)</t>
+  </si>
+  <si>
+    <t>year, feed.unit.value, feed.unit.source, feed.amount.value, feed.amount.source, feed.method.value, feed.method.source, feed.crop_id.value, feed.crop_id.source, feed.additive.value, feed.additive.source, feed.dmi_unit.value, feed.dmi_unit.source, feed.days_on_additive.value, feed.days_on_additive.source, feed.expected_daily_dmi.value, feed.expected_daily_dmi.source</t>
+  </si>
+  <si>
+    <t>json fields(fert_application,data)</t>
+  </si>
+  <si>
+    <t>fert_application is empty, data: year, fert_applications.K.value, fert_applications.K.source, fert_applications.N.value, fert_applications.N.source, fert_applications.P.value, fert_applications.P.source, fert_applications.S.value, fert_applications.S.source, fert_applications.vrt.value, fert_applications.vrt.source, fert_applications.date.value, fert_applications.date.source, fert_applications.unit.value, fert_applications.unit.source, fert_applications.four_r.value, fert_applications.four_r.source, fert_applications.method.value, fert_applications.method.source, fert_applications.crop_id.value, fert_applications.crop_id.source, fert_applications.fert_rate.value, fert_applications.fert_rate.source, fert_applications.inhibitor.value, fert_applications.inhibitor.source, fert_applications.product_type.value, fert_applications.product_type.source, fert_applications.slow_release.value, fert_applications.slow_release.source, fert_applications.management_plan.value, fert_applications.management_plan.source</t>
+  </si>
+  <si>
+    <t>year, seed.type.value, seed.type.source, seed.family.value, seed.family.source, seed.crop_id.value, seed.crop_id.source, seed.plant_date.value, seed.plant_date.source, seed.interseeded.value, seed.interseeded.source</t>
+  </si>
+  <si>
+    <t>year, biomass.crop_id.value, biomass.crop_id.source, biomass.removal_date.value, biomass.removal_date.source, biomass.removal_type.value, biomass.removal_type.source, biomass.percent_removed.value, biomass.percent_removed.source, 
+limings.date.value, limings.date.source, limings.type.value, limings.type.source, limings.amount.value, limings.amount.source, limings.crop_id.value, limings.crop_id.source, 
+grazings.crop_id.value, grazings.crop_id.source, grazings.date_start.value, grazings.date_start.source, grazings.date_end.value, grazings.date_end.source, grazings.grazed_fed.value, grazings.grazed_fed.source, grazings.rest_period.value, grazings.rest_period.source, grazings.feed_ration_type.value, grazings.feed_ration_type.source, grazings.rotational_grazed.value, grazings.rotational_grazed.source, grazings.percent_edible_oil.value, grazings.percent_edible_oil.source, grazings.feed_ration_percent_crude_protein.value, grazings.feed_ration_percent_crude_protein.source, 
+irrigations.unit.value, irrigations.unit.source, irrigations.amount.value, irrigations.amount.source, irrigations.crop_id.value, irrigations.crop_id.source, irrigations.end_date.value, irrigations.end_date.source, irrigations.start_date.value, irrigations.start_date.source, irrigations.method_type.value, irrigations.method_type.source</t>
+  </si>
+  <si>
+    <t>year, soil_sampling.date.value, soil_sampling.date.source, soil_sampling.type.value, soil_sampling.type.source, soil_sampling.crop_id.value, soil_sampling.crop_id.source, soil_sampling.forage_date.value, soil_sampling.forage_date.source, soil_sampling.forage_type.value, soil_sampling.forage_type.source</t>
+  </si>
+  <si>
+    <t>year, stocking.crop_id.value, stocking.crop_id.source, stocking.count_animals.value, stocking.count_animals.source</t>
+  </si>
+  <si>
+    <t>year, crop_protection.date.value, crop_protection.date.source, crop_protection.rate.value, crop_protection.rate.source, crop_protection.type.value, crop_protection.type.source, crop_protection.unit.value, crop_protection.unit.source, crop_protection.method.value, crop_protection.method.source, crop_protection.crop_id.value, crop_protection.crop_id.source, crop_protection.product.value, crop_protection.product.source</t>
+  </si>
+  <si>
+    <t>year, livestock.crop_id.value, livestock.crop_id.source, livestock.species.value, livestock.species.source, livestock.weight_unit.value, livestock.weight_unit.source, livestock.animal_details.value, livestock.animal_details.source, livestock.average_weight.value, livestock.average_weight.source</t>
+  </si>
+  <si>
+    <t>year, conservation.csp.value, conservation.csp.source, conservation.cscg.value, conservation.cscg.source, conservation.rccp.value, conservation.rccp.source, conservation.equip.value, conservation.equip.source, conservation.crop_id.value, conservation.crop_id.source, conservation.carbon_offset.value, conservation.carbon_offset.source, conservation.other_scope_3.value, conservation.other_scope_3.source, conservation.pay_for_practice.value, conservation.pay_for_practice.source, conservation.biodiversity_acres.value, conservation.biodiversity_acres.source</t>
+  </si>
+  <si>
+    <t>cache of pasture_burn and pasture_bqa data</t>
+  </si>
+  <si>
+    <t>year, forage.crop_id.value, forage.crop_id.source, forage.primary_forage.value, forage.primary_forage.source</t>
   </si>
 </sst>
 </file>
@@ -293,12 +344,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,303 +661,404 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.88671875" customWidth="1"/>
     <col min="2" max="2" width="36.21875" customWidth="1"/>
-    <col min="3" max="3" width="45.5546875" customWidth="1"/>
+    <col min="3" max="3" width="64.5546875" customWidth="1"/>
+    <col min="4" max="4" width="60.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
       <c r="C9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
       <c r="C10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
       <c r="C11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
       <c r="C13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
       <c r="C14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
       <c r="C15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
       <c r="C16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
       <c r="C17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
       <c r="C18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
       <c r="C19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
       <c r="C20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
       <c r="C21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
       <c r="C22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
       <c r="C23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
       <c r="C24" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
       <c r="C25" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="D25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
       <c r="C26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="B27" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
       <c r="C29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="B30" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="B32" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="C30" s="2" t="s">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="C32" s="2" t="s">
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>